<commit_message>
added excel reader and creating cards
</commit_message>
<xml_diff>
--- a/server/data/template.xlsx
+++ b/server/data/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1\1\React\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\It\React\StudyProject\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3692BC33-60CB-4C99-BCBA-B5FE1DF58A6F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550F6524-A7A8-4E05-BA69-27929432CE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{9D6708C5-A946-44EC-878F-D823FFA80D20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9D6708C5-A946-44EC-878F-D823FFA80D20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -36,31 +36,61 @@
     <t>Tags</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>tag1</t>
-  </si>
-  <si>
-    <t>tag2</t>
-  </si>
-  <si>
-    <t>tag3</t>
-  </si>
-  <si>
-    <t>sfas</t>
-  </si>
-  <si>
-    <t>asfa</t>
-  </si>
-  <si>
-    <t>a;as;sa</t>
+    <t>gkj;t43</t>
+  </si>
+  <si>
+    <t>Gew3</t>
+  </si>
+  <si>
+    <t>2tg</t>
+  </si>
+  <si>
+    <t>hsdgh</t>
+  </si>
+  <si>
+    <t>sh</t>
+  </si>
+  <si>
+    <t>ghf</t>
+  </si>
+  <si>
+    <t>sgsfsf</t>
+  </si>
+  <si>
+    <t>sfgs</t>
+  </si>
+  <si>
+    <t>fgaf</t>
+  </si>
+  <si>
+    <t>dg3</t>
+  </si>
+  <si>
+    <t>GDF</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>FGADF</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GAGADF</t>
+  </si>
+  <si>
+    <t>FSDg</t>
+  </si>
+  <si>
+    <t>afgd</t>
+  </si>
+  <si>
+    <t>gdfeR</t>
+  </si>
+  <si>
+    <t>RWQ`</t>
   </si>
 </sst>
 </file>
@@ -423,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716C9F4F-3B90-43EB-8749-B54D045BA5F9}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,32 +481,76 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>124</v>
+      </c>
+      <c r="C8">
+        <v>4234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>